<commit_message>
Agrego ejemplos de asignacion multiple con expresion
Para resolverlo se me ocurre que tendria que apilar todos los id que recibo y al final ir asignandolos.
Tambien deberia guardar las posiciones de inicio y fin de la expresion para recorrerlo y reinsertar esos token en la lista cada vez que desapilo un ID.
</commit_message>
<xml_diff>
--- a/Segunda_entrega_correccion/CHECK.xlsx
+++ b/Segunda_entrega_correccion/CHECK.xlsx
@@ -672,7 +672,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1404" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1418" uniqueCount="335">
   <si>
     <t>CELDA 1</t>
   </si>
@@ -1672,6 +1672,12 @@
   </si>
   <si>
     <t>CELDA 272</t>
+  </si>
+  <si>
+    <t>a:=b:=i:=8+5</t>
+  </si>
+  <si>
+    <t>ASIGNACION MULTIPLE CON EXPRESION</t>
   </si>
 </sst>
 </file>
@@ -1967,7 +1973,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2088,14 +2094,23 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2106,6 +2121,15 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2115,37 +2139,16 @@
     <xf numFmtId="0" fontId="1" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2157,22 +2160,49 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2184,9 +2214,6 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2196,74 +2223,32 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <b/>
@@ -2618,7 +2603,7 @@
   <dimension ref="A1:H261"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
-      <selection activeCell="C226" sqref="C226"/>
+      <selection activeCell="I225" sqref="I225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2654,7 +2639,7 @@
       <c r="C2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="56" t="s">
+      <c r="D2" s="59" t="s">
         <v>54</v>
       </c>
       <c r="E2" s="6" t="str">
@@ -2666,7 +2651,7 @@
       </c>
       <c r="H2" s="4">
         <f>COUNTIF(E:E,"ERROR")</f>
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2679,7 +2664,7 @@
       <c r="C3" s="7">
         <v>1</v>
       </c>
-      <c r="D3" s="56"/>
+      <c r="D3" s="59"/>
       <c r="E3" s="6" t="str">
         <f t="shared" ref="E3:E66" si="0">IF(AND(B3=C3,B3&lt;&gt;" "),"OK","ERROR")</f>
         <v>OK</v>
@@ -2695,7 +2680,7 @@
       <c r="C4" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="56"/>
+      <c r="D4" s="59"/>
       <c r="E4" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2711,7 +2696,7 @@
       <c r="C5" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="56" t="s">
+      <c r="D5" s="59" t="s">
         <v>54</v>
       </c>
       <c r="E5" s="6" t="str">
@@ -2729,7 +2714,7 @@
       <c r="C6" s="7">
         <v>10</v>
       </c>
-      <c r="D6" s="56"/>
+      <c r="D6" s="59"/>
       <c r="E6" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2745,7 +2730,7 @@
       <c r="C7" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="56"/>
+      <c r="D7" s="59"/>
       <c r="E7" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2761,7 +2746,7 @@
       <c r="C8" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="63" t="s">
+      <c r="D8" s="60" t="s">
         <v>280</v>
       </c>
       <c r="E8" s="6" t="str">
@@ -2779,7 +2764,7 @@
       <c r="C9" s="7">
         <v>15</v>
       </c>
-      <c r="D9" s="63"/>
+      <c r="D9" s="60"/>
       <c r="E9" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2795,7 +2780,7 @@
       <c r="C10" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="63"/>
+      <c r="D10" s="60"/>
       <c r="E10" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2811,7 +2796,7 @@
       <c r="C11" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="63"/>
+      <c r="D11" s="60"/>
       <c r="E11" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2827,7 +2812,7 @@
       <c r="C12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="63"/>
+      <c r="D12" s="60"/>
       <c r="E12" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2843,7 +2828,7 @@
       <c r="C13" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="63"/>
+      <c r="D13" s="60"/>
       <c r="E13" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2859,7 +2844,7 @@
       <c r="C14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="63"/>
+      <c r="D14" s="60"/>
       <c r="E14" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2875,7 +2860,7 @@
       <c r="C15" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="63"/>
+      <c r="D15" s="60"/>
       <c r="E15" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2891,7 +2876,7 @@
       <c r="C16" s="7">
         <v>16</v>
       </c>
-      <c r="D16" s="63"/>
+      <c r="D16" s="60"/>
       <c r="E16" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2907,7 +2892,7 @@
       <c r="C17" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="63"/>
+      <c r="D17" s="60"/>
       <c r="E17" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2923,7 +2908,7 @@
       <c r="C18" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="63"/>
+      <c r="D18" s="60"/>
       <c r="E18" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2939,7 +2924,7 @@
       <c r="C19" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="63"/>
+      <c r="D19" s="60"/>
       <c r="E19" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2955,7 +2940,7 @@
       <c r="C20" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="58" t="s">
+      <c r="D20" s="61" t="s">
         <v>281</v>
       </c>
       <c r="E20" s="6" t="str">
@@ -2973,7 +2958,7 @@
       <c r="C21" s="7">
         <v>15</v>
       </c>
-      <c r="D21" s="59"/>
+      <c r="D21" s="62"/>
       <c r="E21" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -2989,7 +2974,7 @@
       <c r="C22" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="59"/>
+      <c r="D22" s="62"/>
       <c r="E22" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3005,7 +2990,7 @@
       <c r="C23" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="59"/>
+      <c r="D23" s="62"/>
       <c r="E23" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3021,7 +3006,7 @@
       <c r="C24" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="59"/>
+      <c r="D24" s="62"/>
       <c r="E24" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3037,7 +3022,7 @@
       <c r="C25" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="59"/>
+      <c r="D25" s="62"/>
       <c r="E25" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3053,7 +3038,7 @@
       <c r="C26" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="59"/>
+      <c r="D26" s="62"/>
       <c r="E26" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3069,7 +3054,7 @@
       <c r="C27" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="59"/>
+      <c r="D27" s="62"/>
       <c r="E27" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3085,7 +3070,7 @@
       <c r="C28" s="7">
         <v>16</v>
       </c>
-      <c r="D28" s="59"/>
+      <c r="D28" s="62"/>
       <c r="E28" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3101,7 +3086,7 @@
       <c r="C29" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="59"/>
+      <c r="D29" s="62"/>
       <c r="E29" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3117,7 +3102,7 @@
       <c r="C30" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="59"/>
+      <c r="D30" s="62"/>
       <c r="E30" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3133,7 +3118,7 @@
       <c r="C31" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D31" s="59"/>
+      <c r="D31" s="62"/>
       <c r="E31" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3149,7 +3134,7 @@
       <c r="C32" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="59"/>
+      <c r="D32" s="62"/>
       <c r="E32" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3165,7 +3150,7 @@
       <c r="C33" s="7">
         <v>17</v>
       </c>
-      <c r="D33" s="59"/>
+      <c r="D33" s="62"/>
       <c r="E33" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3181,7 +3166,7 @@
       <c r="C34" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="59"/>
+      <c r="D34" s="62"/>
       <c r="E34" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3197,7 +3182,7 @@
       <c r="C35" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D35" s="63" t="s">
+      <c r="D35" s="60" t="s">
         <v>290</v>
       </c>
       <c r="E35" s="6" t="str">
@@ -3215,7 +3200,7 @@
       <c r="C36" s="7">
         <v>15</v>
       </c>
-      <c r="D36" s="64"/>
+      <c r="D36" s="63"/>
       <c r="E36" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3231,7 +3216,7 @@
       <c r="C37" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D37" s="64"/>
+      <c r="D37" s="63"/>
       <c r="E37" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3247,7 +3232,7 @@
       <c r="C38" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D38" s="64"/>
+      <c r="D38" s="63"/>
       <c r="E38" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3263,7 +3248,7 @@
       <c r="C39" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D39" s="64"/>
+      <c r="D39" s="63"/>
       <c r="E39" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3279,7 +3264,7 @@
       <c r="C40" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D40" s="64"/>
+      <c r="D40" s="63"/>
       <c r="E40" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3295,7 +3280,7 @@
       <c r="C41" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D41" s="64"/>
+      <c r="D41" s="63"/>
       <c r="E41" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3311,7 +3296,7 @@
       <c r="C42" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D42" s="64"/>
+      <c r="D42" s="63"/>
       <c r="E42" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3327,7 +3312,7 @@
       <c r="C43" s="7">
         <v>4</v>
       </c>
-      <c r="D43" s="64"/>
+      <c r="D43" s="63"/>
       <c r="E43" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3343,7 +3328,7 @@
       <c r="C44" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D44" s="64"/>
+      <c r="D44" s="63"/>
       <c r="E44" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3359,7 +3344,7 @@
       <c r="C45" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D45" s="64"/>
+      <c r="D45" s="63"/>
       <c r="E45" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3375,7 +3360,7 @@
       <c r="C46" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D46" s="64"/>
+      <c r="D46" s="63"/>
       <c r="E46" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3391,7 +3376,7 @@
       <c r="C47" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D47" s="64"/>
+      <c r="D47" s="63"/>
       <c r="E47" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3408,7 +3393,7 @@
       <c r="C48" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D48" s="64"/>
+      <c r="D48" s="63"/>
       <c r="E48" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3425,7 +3410,7 @@
       <c r="C49" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D49" s="64"/>
+      <c r="D49" s="63"/>
       <c r="E49" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3442,7 +3427,7 @@
       <c r="C50" s="7">
         <v>16</v>
       </c>
-      <c r="D50" s="64"/>
+      <c r="D50" s="63"/>
       <c r="E50" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3459,7 +3444,7 @@
       <c r="C51" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D51" s="64"/>
+      <c r="D51" s="63"/>
       <c r="E51" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3475,7 +3460,7 @@
       <c r="C52" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D52" s="64"/>
+      <c r="D52" s="63"/>
       <c r="E52" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3491,7 +3476,7 @@
       <c r="C53" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D53" s="64"/>
+      <c r="D53" s="63"/>
       <c r="E53" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3507,7 +3492,7 @@
       <c r="C54" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="D54" s="64"/>
+      <c r="D54" s="63"/>
       <c r="E54" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3523,7 +3508,7 @@
       <c r="C55" s="7">
         <v>17</v>
       </c>
-      <c r="D55" s="64"/>
+      <c r="D55" s="63"/>
       <c r="E55" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3539,7 +3524,7 @@
       <c r="C56" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D56" s="64"/>
+      <c r="D56" s="63"/>
       <c r="E56" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3555,7 +3540,7 @@
       <c r="C57" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D57" s="65" t="s">
+      <c r="D57" s="64" t="s">
         <v>291</v>
       </c>
       <c r="E57" s="6" t="str">
@@ -3573,7 +3558,7 @@
       <c r="C58" s="7">
         <v>15</v>
       </c>
-      <c r="D58" s="66"/>
+      <c r="D58" s="65"/>
       <c r="E58" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3589,7 +3574,7 @@
       <c r="C59" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D59" s="66"/>
+      <c r="D59" s="65"/>
       <c r="E59" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3605,7 +3590,7 @@
       <c r="C60" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D60" s="66"/>
+      <c r="D60" s="65"/>
       <c r="E60" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3621,7 +3606,7 @@
       <c r="C61" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D61" s="66"/>
+      <c r="D61" s="65"/>
       <c r="E61" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3637,7 +3622,7 @@
       <c r="C62" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D62" s="66"/>
+      <c r="D62" s="65"/>
       <c r="E62" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3653,7 +3638,7 @@
       <c r="C63" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D63" s="66"/>
+      <c r="D63" s="65"/>
       <c r="E63" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3669,7 +3654,7 @@
       <c r="C64" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D64" s="66"/>
+      <c r="D64" s="65"/>
       <c r="E64" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3685,7 +3670,7 @@
       <c r="C65" s="7">
         <v>4</v>
       </c>
-      <c r="D65" s="66"/>
+      <c r="D65" s="65"/>
       <c r="E65" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3701,7 +3686,7 @@
       <c r="C66" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D66" s="66"/>
+      <c r="D66" s="65"/>
       <c r="E66" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -3717,7 +3702,7 @@
       <c r="C67" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D67" s="66"/>
+      <c r="D67" s="65"/>
       <c r="E67" s="6" t="str">
         <f t="shared" ref="E67:E136" si="1">IF(AND(B67=C67,B67&lt;&gt;" "),"OK","ERROR")</f>
         <v>OK</v>
@@ -3733,7 +3718,7 @@
       <c r="C68" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D68" s="66"/>
+      <c r="D68" s="65"/>
       <c r="E68" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3749,7 +3734,7 @@
       <c r="C69" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D69" s="66"/>
+      <c r="D69" s="65"/>
       <c r="E69" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3765,7 +3750,7 @@
       <c r="C70" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D70" s="66"/>
+      <c r="D70" s="65"/>
       <c r="E70" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3781,7 +3766,7 @@
       <c r="C71" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D71" s="66"/>
+      <c r="D71" s="65"/>
       <c r="E71" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3797,7 +3782,7 @@
       <c r="C72" s="7">
         <v>16</v>
       </c>
-      <c r="D72" s="66"/>
+      <c r="D72" s="65"/>
       <c r="E72" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3813,7 +3798,7 @@
       <c r="C73" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D73" s="66"/>
+      <c r="D73" s="65"/>
       <c r="E73" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3829,7 +3814,7 @@
       <c r="C74" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D74" s="66"/>
+      <c r="D74" s="65"/>
       <c r="E74" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3845,7 +3830,7 @@
       <c r="C75" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D75" s="66"/>
+      <c r="D75" s="65"/>
       <c r="E75" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3861,7 +3846,7 @@
       <c r="C76" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D76" s="66"/>
+      <c r="D76" s="65"/>
       <c r="E76" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3877,7 +3862,7 @@
       <c r="C77" s="7">
         <v>17</v>
       </c>
-      <c r="D77" s="66"/>
+      <c r="D77" s="65"/>
       <c r="E77" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3893,7 +3878,7 @@
       <c r="C78" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D78" s="66"/>
+      <c r="D78" s="65"/>
       <c r="E78" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3909,7 +3894,7 @@
       <c r="C79" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D79" s="70" t="s">
+      <c r="D79" s="66" t="s">
         <v>295</v>
       </c>
       <c r="E79" s="6" t="str">
@@ -3927,7 +3912,7 @@
       <c r="C80" s="7">
         <v>7</v>
       </c>
-      <c r="D80" s="71"/>
+      <c r="D80" s="67"/>
       <c r="E80" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3943,7 +3928,7 @@
       <c r="C81" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D81" s="71"/>
+      <c r="D81" s="67"/>
       <c r="E81" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3959,7 +3944,7 @@
       <c r="C82" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D82" s="71"/>
+      <c r="D82" s="67"/>
       <c r="E82" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3975,7 +3960,7 @@
       <c r="C83" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="D83" s="71"/>
+      <c r="D83" s="67"/>
       <c r="E83" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -3991,7 +3976,7 @@
       <c r="C84" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D84" s="71"/>
+      <c r="D84" s="67"/>
       <c r="E84" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4007,7 +3992,7 @@
       <c r="C85" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="D85" s="71"/>
+      <c r="D85" s="67"/>
       <c r="E85" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4023,7 +4008,7 @@
       <c r="C86" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D86" s="71"/>
+      <c r="D86" s="67"/>
       <c r="E86" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4039,7 +4024,7 @@
       <c r="C87" s="7">
         <v>5</v>
       </c>
-      <c r="D87" s="71"/>
+      <c r="D87" s="67"/>
       <c r="E87" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4055,7 +4040,7 @@
       <c r="C88" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D88" s="71"/>
+      <c r="D88" s="67"/>
       <c r="E88" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4071,7 +4056,7 @@
       <c r="C89" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D89" s="71"/>
+      <c r="D89" s="67"/>
       <c r="E89" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4081,13 +4066,13 @@
       <c r="A90" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="B90" s="88" t="s">
+      <c r="B90" s="45" t="s">
         <v>33</v>
       </c>
       <c r="C90" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D90" s="87"/>
+      <c r="D90" s="68"/>
       <c r="E90" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4103,7 +4088,7 @@
       <c r="C91" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D91" s="71"/>
+      <c r="D91" s="67"/>
       <c r="E91" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4119,7 +4104,7 @@
       <c r="C92" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D92" s="72"/>
+      <c r="D92" s="69"/>
       <c r="E92" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4135,7 +4120,7 @@
       <c r="C93" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D93" s="58" t="s">
+      <c r="D93" s="61" t="s">
         <v>296</v>
       </c>
       <c r="E93" s="6" t="str">
@@ -4153,7 +4138,7 @@
       <c r="C94" s="7">
         <v>7</v>
       </c>
-      <c r="D94" s="59"/>
+      <c r="D94" s="62"/>
       <c r="E94" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4169,7 +4154,7 @@
       <c r="C95" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D95" s="59"/>
+      <c r="D95" s="62"/>
       <c r="E95" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4185,7 +4170,7 @@
       <c r="C96" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D96" s="59"/>
+      <c r="D96" s="62"/>
       <c r="E96" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4201,7 +4186,7 @@
       <c r="C97" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="D97" s="59"/>
+      <c r="D97" s="62"/>
       <c r="E97" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4217,7 +4202,7 @@
       <c r="C98" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D98" s="59"/>
+      <c r="D98" s="62"/>
       <c r="E98" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4233,7 +4218,7 @@
       <c r="C99" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="D99" s="59"/>
+      <c r="D99" s="62"/>
       <c r="E99" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4249,7 +4234,7 @@
       <c r="C100" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D100" s="59"/>
+      <c r="D100" s="62"/>
       <c r="E100" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4265,7 +4250,7 @@
       <c r="C101" s="7">
         <v>8</v>
       </c>
-      <c r="D101" s="59"/>
+      <c r="D101" s="62"/>
       <c r="E101" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4281,7 +4266,7 @@
       <c r="C102" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D102" s="59"/>
+      <c r="D102" s="62"/>
       <c r="E102" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4297,7 +4282,7 @@
       <c r="C103" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D103" s="59"/>
+      <c r="D103" s="62"/>
       <c r="E103" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4313,7 +4298,7 @@
       <c r="C104" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="D104" s="59"/>
+      <c r="D104" s="62"/>
       <c r="E104" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4329,7 +4314,7 @@
       <c r="C105" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D105" s="59"/>
+      <c r="D105" s="62"/>
       <c r="E105" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4345,7 +4330,7 @@
       <c r="C106" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="D106" s="59"/>
+      <c r="D106" s="62"/>
       <c r="E106" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4361,7 +4346,7 @@
       <c r="C107" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D107" s="59"/>
+      <c r="D107" s="62"/>
       <c r="E107" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4377,7 +4362,7 @@
       <c r="C108" s="7">
         <v>5</v>
       </c>
-      <c r="D108" s="59"/>
+      <c r="D108" s="62"/>
       <c r="E108" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4393,7 +4378,7 @@
       <c r="C109" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D109" s="59"/>
+      <c r="D109" s="62"/>
       <c r="E109" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4409,7 +4394,7 @@
       <c r="C110" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D110" s="59"/>
+      <c r="D110" s="62"/>
       <c r="E110" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4425,7 +4410,7 @@
       <c r="C111" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D111" s="59"/>
+      <c r="D111" s="62"/>
       <c r="E111" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4441,7 +4426,7 @@
       <c r="C112" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="D112" s="89"/>
+      <c r="D112" s="70"/>
       <c r="E112" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4457,7 +4442,7 @@
       <c r="C113" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="D113" s="59"/>
+      <c r="D113" s="62"/>
       <c r="E113" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4467,13 +4452,13 @@
       <c r="A114" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B114" s="91" t="s">
+      <c r="B114" s="46" t="s">
         <v>28</v>
       </c>
       <c r="C114" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="D114" s="92" t="s">
+      <c r="D114" s="71" t="s">
         <v>297</v>
       </c>
       <c r="E114" s="6" t="str">
@@ -4491,7 +4476,7 @@
       <c r="C115" s="7">
         <v>7</v>
       </c>
-      <c r="D115" s="61"/>
+      <c r="D115" s="72"/>
       <c r="E115" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4507,7 +4492,7 @@
       <c r="C116" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D116" s="61"/>
+      <c r="D116" s="72"/>
       <c r="E116" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4523,7 +4508,7 @@
       <c r="C117" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D117" s="61"/>
+      <c r="D117" s="72"/>
       <c r="E117" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4539,7 +4524,7 @@
       <c r="C118" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="D118" s="61"/>
+      <c r="D118" s="72"/>
       <c r="E118" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4555,7 +4540,7 @@
       <c r="C119" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D119" s="61"/>
+      <c r="D119" s="72"/>
       <c r="E119" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4571,7 +4556,7 @@
       <c r="C120" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="D120" s="61"/>
+      <c r="D120" s="72"/>
       <c r="E120" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4587,7 +4572,7 @@
       <c r="C121" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D121" s="61"/>
+      <c r="D121" s="72"/>
       <c r="E121" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4603,7 +4588,7 @@
       <c r="C122" s="7">
         <v>8</v>
       </c>
-      <c r="D122" s="61"/>
+      <c r="D122" s="72"/>
       <c r="E122" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4619,7 +4604,7 @@
       <c r="C123" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D123" s="61"/>
+      <c r="D123" s="72"/>
       <c r="E123" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4635,7 +4620,7 @@
       <c r="C124" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D124" s="61"/>
+      <c r="D124" s="72"/>
       <c r="E124" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4651,7 +4636,7 @@
       <c r="C125" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="D125" s="61"/>
+      <c r="D125" s="72"/>
       <c r="E125" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4667,7 +4652,7 @@
       <c r="C126" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D126" s="61"/>
+      <c r="D126" s="72"/>
       <c r="E126" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4683,7 +4668,7 @@
       <c r="C127" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="D127" s="61"/>
+      <c r="D127" s="72"/>
       <c r="E127" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4699,7 +4684,7 @@
       <c r="C128" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D128" s="61"/>
+      <c r="D128" s="72"/>
       <c r="E128" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4715,7 +4700,7 @@
       <c r="C129" s="7">
         <v>5</v>
       </c>
-      <c r="D129" s="61"/>
+      <c r="D129" s="72"/>
       <c r="E129" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4731,7 +4716,7 @@
       <c r="C130" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D130" s="61"/>
+      <c r="D130" s="72"/>
       <c r="E130" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4747,7 +4732,7 @@
       <c r="C131" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D131" s="61"/>
+      <c r="D131" s="72"/>
       <c r="E131" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4763,7 +4748,7 @@
       <c r="C132" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D132" s="61"/>
+      <c r="D132" s="72"/>
       <c r="E132" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4773,13 +4758,13 @@
       <c r="A133" s="38" t="s">
         <v>145</v>
       </c>
-      <c r="B133" s="88" t="s">
+      <c r="B133" s="45" t="s">
         <v>36</v>
       </c>
       <c r="C133" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D133" s="90"/>
+      <c r="D133" s="73"/>
       <c r="E133" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4795,7 +4780,7 @@
       <c r="C134" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="D134" s="62"/>
+      <c r="D134" s="74"/>
       <c r="E134" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4811,7 +4796,7 @@
       <c r="C135" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D135" s="47" t="s">
+      <c r="D135" s="50" t="s">
         <v>302</v>
       </c>
       <c r="E135" s="6" t="str">
@@ -4829,7 +4814,7 @@
       <c r="C136" s="7">
         <v>8</v>
       </c>
-      <c r="D136" s="48"/>
+      <c r="D136" s="51"/>
       <c r="E136" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -4845,7 +4830,7 @@
       <c r="C137" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D137" s="48"/>
+      <c r="D137" s="51"/>
       <c r="E137" s="6" t="str">
         <f t="shared" ref="E137:E143" si="2">IF(AND(B137=C137,B137&lt;&gt;" "),"OK","ERROR")</f>
         <v>OK</v>
@@ -4861,7 +4846,7 @@
       <c r="C138" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D138" s="48"/>
+      <c r="D138" s="51"/>
       <c r="E138" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -4877,7 +4862,7 @@
       <c r="C139" s="7">
         <v>8</v>
       </c>
-      <c r="D139" s="48"/>
+      <c r="D139" s="51"/>
       <c r="E139" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -4893,7 +4878,7 @@
       <c r="C140" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D140" s="48"/>
+      <c r="D140" s="51"/>
       <c r="E140" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -4909,7 +4894,7 @@
       <c r="C141" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D141" s="48"/>
+      <c r="D141" s="51"/>
       <c r="E141" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -4925,7 +4910,7 @@
       <c r="C142" s="7">
         <v>8</v>
       </c>
-      <c r="D142" s="48"/>
+      <c r="D142" s="51"/>
       <c r="E142" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -4941,7 +4926,7 @@
       <c r="C143" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D143" s="49"/>
+      <c r="D143" s="52"/>
       <c r="E143" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -4957,7 +4942,7 @@
       <c r="C144" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D144" s="50" t="s">
+      <c r="D144" s="56" t="s">
         <v>307</v>
       </c>
       <c r="E144" s="6" t="str">
@@ -4975,7 +4960,7 @@
       <c r="C145" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D145" s="51"/>
+      <c r="D145" s="57"/>
       <c r="E145" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -4991,7 +4976,7 @@
       <c r="C146" s="7">
         <v>2</v>
       </c>
-      <c r="D146" s="51"/>
+      <c r="D146" s="57"/>
       <c r="E146" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5007,7 +4992,7 @@
       <c r="C147" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D147" s="51"/>
+      <c r="D147" s="57"/>
       <c r="E147" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5023,7 +5008,7 @@
       <c r="C148" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="D148" s="51"/>
+      <c r="D148" s="57"/>
       <c r="E148" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5039,7 +5024,7 @@
       <c r="C149" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="D149" s="51"/>
+      <c r="D149" s="57"/>
       <c r="E149" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5055,7 +5040,7 @@
       <c r="C150" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D150" s="51"/>
+      <c r="D150" s="57"/>
       <c r="E150" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5071,7 +5056,7 @@
       <c r="C151" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="D151" s="51"/>
+      <c r="D151" s="57"/>
       <c r="E151" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5087,7 +5072,7 @@
       <c r="C152" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D152" s="51"/>
+      <c r="D152" s="57"/>
       <c r="E152" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5103,7 +5088,7 @@
       <c r="C153" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D153" s="51"/>
+      <c r="D153" s="57"/>
       <c r="E153" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5119,7 +5104,7 @@
       <c r="C154" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D154" s="51"/>
+      <c r="D154" s="57"/>
       <c r="E154" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5135,7 +5120,7 @@
       <c r="C155" s="7">
         <v>4</v>
       </c>
-      <c r="D155" s="51"/>
+      <c r="D155" s="57"/>
       <c r="E155" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5151,7 +5136,7 @@
       <c r="C156" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D156" s="51"/>
+      <c r="D156" s="57"/>
       <c r="E156" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5167,7 +5152,7 @@
       <c r="C157" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="D157" s="51"/>
+      <c r="D157" s="57"/>
       <c r="E157" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5183,7 +5168,7 @@
       <c r="C158" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D158" s="51"/>
+      <c r="D158" s="57"/>
       <c r="E158" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5199,7 +5184,7 @@
       <c r="C159" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="D159" s="51"/>
+      <c r="D159" s="57"/>
       <c r="E159" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5215,7 +5200,7 @@
       <c r="C160" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="D160" s="51"/>
+      <c r="D160" s="57"/>
       <c r="E160" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5231,7 +5216,7 @@
       <c r="C161" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D161" s="51"/>
+      <c r="D161" s="57"/>
       <c r="E161" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5247,7 +5232,7 @@
       <c r="C162" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="D162" s="51"/>
+      <c r="D162" s="57"/>
       <c r="E162" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5263,7 +5248,7 @@
       <c r="C163" s="7">
         <v>1</v>
       </c>
-      <c r="D163" s="51"/>
+      <c r="D163" s="57"/>
       <c r="E163" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5279,7 +5264,7 @@
       <c r="C164" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D164" s="51"/>
+      <c r="D164" s="57"/>
       <c r="E164" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5295,7 +5280,7 @@
       <c r="C165" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="D165" s="51"/>
+      <c r="D165" s="57"/>
       <c r="E165" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5311,7 +5296,7 @@
       <c r="C166" s="35">
         <v>0</v>
       </c>
-      <c r="D166" s="52"/>
+      <c r="D166" s="58"/>
       <c r="E166" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5327,7 +5312,7 @@
       <c r="C167" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="D167" s="53" t="s">
+      <c r="D167" s="47" t="s">
         <v>322</v>
       </c>
       <c r="E167" s="6" t="str">
@@ -5345,7 +5330,7 @@
       <c r="C168" s="7">
         <v>1</v>
       </c>
-      <c r="D168" s="54"/>
+      <c r="D168" s="48"/>
       <c r="E168" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5361,7 +5346,7 @@
       <c r="C169" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D169" s="55"/>
+      <c r="D169" s="49"/>
       <c r="E169" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5377,7 +5362,7 @@
       <c r="C170" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="D170" s="47" t="s">
+      <c r="D170" s="50" t="s">
         <v>322</v>
       </c>
       <c r="E170" s="6" t="str">
@@ -5395,7 +5380,7 @@
       <c r="C171" s="7">
         <v>15</v>
       </c>
-      <c r="D171" s="48"/>
+      <c r="D171" s="51"/>
       <c r="E171" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5411,7 +5396,7 @@
       <c r="C172" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D172" s="49"/>
+      <c r="D172" s="52"/>
       <c r="E172" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5427,7 +5412,7 @@
       <c r="C173" s="37" t="s">
         <v>313</v>
       </c>
-      <c r="D173" s="53" t="s">
+      <c r="D173" s="47" t="s">
         <v>321</v>
       </c>
       <c r="E173" s="6" t="str">
@@ -5445,7 +5430,7 @@
       <c r="C174" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="D174" s="54"/>
+      <c r="D174" s="48"/>
       <c r="E174" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5461,7 +5446,7 @@
       <c r="C175" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D175" s="55"/>
+      <c r="D175" s="49"/>
       <c r="E175" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5477,7 +5462,7 @@
       <c r="C176" s="37" t="s">
         <v>313</v>
       </c>
-      <c r="D176" s="47" t="s">
+      <c r="D176" s="50" t="s">
         <v>321</v>
       </c>
       <c r="E176" s="6" t="str">
@@ -5495,7 +5480,7 @@
       <c r="C177" s="7" t="s">
         <v>315</v>
       </c>
-      <c r="D177" s="48"/>
+      <c r="D177" s="51"/>
       <c r="E177" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5511,7 +5496,7 @@
       <c r="C178" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D178" s="49"/>
+      <c r="D178" s="52"/>
       <c r="E178" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5527,7 +5512,7 @@
       <c r="C179" s="37" t="s">
         <v>313</v>
       </c>
-      <c r="D179" s="53" t="s">
+      <c r="D179" s="47" t="s">
         <v>321</v>
       </c>
       <c r="E179" s="6" t="str">
@@ -5545,7 +5530,7 @@
       <c r="C180" s="7" t="s">
         <v>316</v>
       </c>
-      <c r="D180" s="54"/>
+      <c r="D180" s="48"/>
       <c r="E180" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5561,7 +5546,7 @@
       <c r="C181" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D181" s="55"/>
+      <c r="D181" s="49"/>
       <c r="E181" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5577,7 +5562,7 @@
       <c r="C182" s="37" t="s">
         <v>313</v>
       </c>
-      <c r="D182" s="47" t="s">
+      <c r="D182" s="50" t="s">
         <v>320</v>
       </c>
       <c r="E182" s="6" t="str">
@@ -5595,7 +5580,7 @@
       <c r="C183" s="7" t="s">
         <v>317</v>
       </c>
-      <c r="D183" s="48"/>
+      <c r="D183" s="51"/>
       <c r="E183" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5611,7 +5596,7 @@
       <c r="C184" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D184" s="49"/>
+      <c r="D184" s="52"/>
       <c r="E184" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5627,7 +5612,7 @@
       <c r="C185" s="37" t="s">
         <v>318</v>
       </c>
-      <c r="D185" s="53" t="s">
+      <c r="D185" s="47" t="s">
         <v>319</v>
       </c>
       <c r="E185" s="6" t="str">
@@ -5640,7 +5625,7 @@
         <v>198</v>
       </c>
       <c r="B186" s="9"/>
-      <c r="D186" s="54"/>
+      <c r="D186" s="48"/>
       <c r="E186" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5656,7 +5641,7 @@
       <c r="C187" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D187" s="55"/>
+      <c r="D187" s="49"/>
       <c r="E187" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5672,7 +5657,7 @@
       <c r="C188" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="D188" s="67" t="s">
+      <c r="D188" s="53" t="s">
         <v>326</v>
       </c>
       <c r="E188" s="6" t="str">
@@ -5690,7 +5675,7 @@
       <c r="C189" s="7">
         <v>2</v>
       </c>
-      <c r="D189" s="68"/>
+      <c r="D189" s="54"/>
       <c r="E189" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5706,7 +5691,7 @@
       <c r="C190" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D190" s="68"/>
+      <c r="D190" s="54"/>
       <c r="E190" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5722,7 +5707,7 @@
       <c r="C191" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="D191" s="68"/>
+      <c r="D191" s="54"/>
       <c r="E191" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5738,7 +5723,7 @@
       <c r="C192" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="D192" s="68"/>
+      <c r="D192" s="54"/>
       <c r="E192" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5754,7 +5739,7 @@
       <c r="C193" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D193" s="68"/>
+      <c r="D193" s="54"/>
       <c r="E193" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5770,7 +5755,7 @@
       <c r="C194" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="D194" s="68"/>
+      <c r="D194" s="54"/>
       <c r="E194" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5786,7 +5771,7 @@
       <c r="C195" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D195" s="68"/>
+      <c r="D195" s="54"/>
       <c r="E195" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5802,7 +5787,7 @@
       <c r="C196" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D196" s="68"/>
+      <c r="D196" s="54"/>
       <c r="E196" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5818,7 +5803,7 @@
       <c r="C197" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D197" s="68"/>
+      <c r="D197" s="54"/>
       <c r="E197" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5834,7 +5819,7 @@
       <c r="C198" s="7">
         <v>4</v>
       </c>
-      <c r="D198" s="68"/>
+      <c r="D198" s="54"/>
       <c r="E198" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5850,7 +5835,7 @@
       <c r="C199" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D199" s="68"/>
+      <c r="D199" s="54"/>
       <c r="E199" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5866,7 +5851,7 @@
       <c r="C200" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="D200" s="68"/>
+      <c r="D200" s="54"/>
       <c r="E200" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5882,7 +5867,7 @@
       <c r="C201" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D201" s="68"/>
+      <c r="D201" s="54"/>
       <c r="E201" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5898,7 +5883,7 @@
       <c r="C202" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="D202" s="68"/>
+      <c r="D202" s="54"/>
       <c r="E202" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5914,7 +5899,7 @@
       <c r="C203" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="D203" s="68"/>
+      <c r="D203" s="54"/>
       <c r="E203" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5930,7 +5915,7 @@
       <c r="C204" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D204" s="68"/>
+      <c r="D204" s="54"/>
       <c r="E204" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5946,7 +5931,7 @@
       <c r="C205" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="D205" s="68"/>
+      <c r="D205" s="54"/>
       <c r="E205" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5962,7 +5947,7 @@
       <c r="C206" s="7">
         <v>1</v>
       </c>
-      <c r="D206" s="68"/>
+      <c r="D206" s="54"/>
       <c r="E206" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5978,7 +5963,7 @@
       <c r="C207" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D207" s="68"/>
+      <c r="D207" s="54"/>
       <c r="E207" s="6" t="str">
         <f t="shared" si="3"/>
         <v>OK</v>
@@ -5994,7 +5979,7 @@
       <c r="C208" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="D208" s="68"/>
+      <c r="D208" s="54"/>
       <c r="E208" s="6" t="str">
         <f t="shared" ref="E208:E259" si="4">IF(AND(B208=C208,B208&lt;&gt;" "),"OK","ERROR")</f>
         <v>OK</v>
@@ -6010,7 +5995,7 @@
       <c r="C209" s="7">
         <v>0</v>
       </c>
-      <c r="D209" s="68"/>
+      <c r="D209" s="54"/>
       <c r="E209" s="6" t="str">
         <f t="shared" si="4"/>
         <v>OK</v>
@@ -6026,7 +6011,7 @@
       <c r="C210" s="7">
         <v>1</v>
       </c>
-      <c r="D210" s="68"/>
+      <c r="D210" s="54"/>
       <c r="E210" s="6" t="str">
         <f t="shared" si="4"/>
         <v>OK</v>
@@ -6042,7 +6027,7 @@
       <c r="C211" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D211" s="68"/>
+      <c r="D211" s="54"/>
       <c r="E211" s="6" t="str">
         <f t="shared" si="4"/>
         <v>OK</v>
@@ -6058,7 +6043,7 @@
       <c r="C212" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D212" s="68"/>
+      <c r="D212" s="54"/>
       <c r="E212" s="6" t="str">
         <f t="shared" si="4"/>
         <v>OK</v>
@@ -6074,7 +6059,7 @@
       <c r="C213" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="D213" s="68"/>
+      <c r="D213" s="54"/>
       <c r="E213" s="6" t="str">
         <f t="shared" si="4"/>
         <v>OK</v>
@@ -6090,7 +6075,7 @@
       <c r="C214" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D214" s="68"/>
+      <c r="D214" s="54"/>
       <c r="E214" s="6" t="str">
         <f t="shared" si="4"/>
         <v>OK</v>
@@ -6106,7 +6091,7 @@
       <c r="C215" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="D215" s="68"/>
+      <c r="D215" s="54"/>
       <c r="E215" s="6" t="str">
         <f t="shared" si="4"/>
         <v>OK</v>
@@ -6122,7 +6107,7 @@
       <c r="C216" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D216" s="68"/>
+      <c r="D216" s="54"/>
       <c r="E216" s="6" t="str">
         <f t="shared" si="4"/>
         <v>OK</v>
@@ -6138,7 +6123,7 @@
       <c r="C217" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D217" s="68"/>
+      <c r="D217" s="54"/>
       <c r="E217" s="6" t="str">
         <f t="shared" si="4"/>
         <v>OK</v>
@@ -6154,7 +6139,7 @@
       <c r="C218" s="7">
         <v>2</v>
       </c>
-      <c r="D218" s="68"/>
+      <c r="D218" s="54"/>
       <c r="E218" s="6" t="str">
         <f t="shared" si="4"/>
         <v>OK</v>
@@ -6170,7 +6155,7 @@
       <c r="C219" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D219" s="68"/>
+      <c r="D219" s="54"/>
       <c r="E219" s="6" t="str">
         <f t="shared" si="4"/>
         <v>OK</v>
@@ -6186,7 +6171,7 @@
       <c r="C220" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D220" s="68"/>
+      <c r="D220" s="54"/>
       <c r="E220" s="6" t="str">
         <f t="shared" si="4"/>
         <v>OK</v>
@@ -6202,7 +6187,7 @@
       <c r="C221" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D221" s="68"/>
+      <c r="D221" s="54"/>
       <c r="E221" s="6" t="str">
         <f t="shared" si="4"/>
         <v>OK</v>
@@ -6218,7 +6203,7 @@
       <c r="C222" s="35" t="s">
         <v>235</v>
       </c>
-      <c r="D222" s="69"/>
+      <c r="D222" s="55"/>
       <c r="E222" s="6" t="str">
         <f t="shared" si="4"/>
         <v>OK</v>
@@ -6228,117 +6213,159 @@
       <c r="A223" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="D223" s="44"/>
+      <c r="B223" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D223" s="91" t="s">
+        <v>334</v>
+      </c>
       <c r="E223" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>OK</v>
+        <v>ERROR</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="D224" s="44"/>
+      <c r="B224" s="8">
+        <v>8</v>
+      </c>
+      <c r="D224" s="92"/>
       <c r="E224" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>OK</v>
+        <v>ERROR</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="B225" s="46"/>
+      <c r="B225" s="44">
+        <v>5</v>
+      </c>
       <c r="C225" s="26"/>
-      <c r="D225" s="44"/>
+      <c r="D225" s="92"/>
       <c r="E225" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>OK</v>
+        <v>ERROR</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="D226" s="44"/>
+      <c r="B226" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D226" s="92"/>
       <c r="E226" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>OK</v>
+        <v>ERROR</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="D227" s="44"/>
+      <c r="B227" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D227" s="92"/>
       <c r="E227" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>OK</v>
+        <v>ERROR</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="B228" s="43"/>
-      <c r="D228" s="45"/>
+      <c r="B228" s="43">
+        <v>8</v>
+      </c>
+      <c r="D228" s="92"/>
       <c r="E228" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>OK</v>
+        <v>ERROR</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="3" t="s">
         <v>253</v>
       </c>
+      <c r="B229" s="8">
+        <v>5</v>
+      </c>
+      <c r="D229" s="92"/>
       <c r="E229" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>OK</v>
+        <v>ERROR</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="3" t="s">
         <v>254</v>
       </c>
+      <c r="B230" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D230" s="92"/>
       <c r="E230" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>OK</v>
+        <v>ERROR</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="3" t="s">
         <v>255</v>
       </c>
+      <c r="B231" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D231" s="92"/>
       <c r="E231" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>OK</v>
+        <v>ERROR</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="3" t="s">
         <v>256</v>
       </c>
+      <c r="B232" s="8">
+        <v>8</v>
+      </c>
+      <c r="D232" s="92"/>
       <c r="E232" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>OK</v>
+        <v>ERROR</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="3" t="s">
         <v>257</v>
       </c>
+      <c r="B233" s="8">
+        <v>5</v>
+      </c>
+      <c r="D233" s="92"/>
       <c r="E233" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>OK</v>
+        <v>ERROR</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="3" t="s">
         <v>258</v>
       </c>
+      <c r="B234" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D234" s="93"/>
       <c r="E234" s="6" t="str">
         <f t="shared" si="4"/>
-        <v>OK</v>
+        <v>ERROR</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
@@ -6585,13 +6612,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="D173:D175"/>
-    <mergeCell ref="D176:D178"/>
-    <mergeCell ref="D188:D222"/>
-    <mergeCell ref="D179:D181"/>
-    <mergeCell ref="D182:D184"/>
-    <mergeCell ref="D185:D187"/>
+  <mergeCells count="20">
+    <mergeCell ref="D223:D234"/>
     <mergeCell ref="D135:D143"/>
     <mergeCell ref="D144:D166"/>
     <mergeCell ref="D167:D169"/>
@@ -6605,6 +6627,12 @@
     <mergeCell ref="D79:D92"/>
     <mergeCell ref="D93:D113"/>
     <mergeCell ref="D114:D134"/>
+    <mergeCell ref="D173:D175"/>
+    <mergeCell ref="D176:D178"/>
+    <mergeCell ref="D188:D222"/>
+    <mergeCell ref="D179:D181"/>
+    <mergeCell ref="D182:D184"/>
+    <mergeCell ref="D185:D187"/>
   </mergeCells>
   <conditionalFormatting sqref="E2:E261">
     <cfRule type="expression" dxfId="3" priority="1">
@@ -6647,25 +6675,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="84" t="s">
+      <c r="B1" s="75" t="s">
         <v>284</v>
       </c>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="85" t="s">
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="76" t="s">
         <v>285</v>
       </c>
-      <c r="J1" s="85"/>
-      <c r="K1" s="85"/>
-      <c r="L1" s="85"/>
-      <c r="M1" s="85"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
     </row>
     <row r="2" spans="1:48" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="77" t="s">
         <v>283</v>
       </c>
       <c r="B2" s="16">
@@ -6811,7 +6839,7 @@
       </c>
     </row>
     <row r="3" spans="1:48" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="76"/>
+      <c r="A3" s="77"/>
       <c r="B3" s="17" t="s">
         <v>32</v>
       </c>
@@ -6885,31 +6913,31 @@
       <c r="AV3" s="17"/>
     </row>
     <row r="4" spans="1:48" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="75" t="s">
         <v>284</v>
       </c>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="85" t="s">
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="76" t="s">
         <v>285</v>
       </c>
-      <c r="J4" s="85"/>
-      <c r="K4" s="85"/>
-      <c r="L4" s="85"/>
-      <c r="M4" s="85"/>
-      <c r="N4" s="83" t="s">
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
+      <c r="L4" s="76"/>
+      <c r="M4" s="76"/>
+      <c r="N4" s="87" t="s">
         <v>287</v>
       </c>
-      <c r="O4" s="83"/>
-      <c r="P4" s="83"/>
-      <c r="Q4" s="83"/>
+      <c r="O4" s="87"/>
+      <c r="P4" s="87"/>
+      <c r="Q4" s="87"/>
     </row>
     <row r="5" spans="1:48" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="76" t="s">
+      <c r="A5" s="77" t="s">
         <v>286</v>
       </c>
       <c r="B5" s="16">
@@ -7055,7 +7083,7 @@
       </c>
     </row>
     <row r="6" spans="1:48" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="76"/>
+      <c r="A6" s="77"/>
       <c r="B6" s="17" t="s">
         <v>32</v>
       </c>
@@ -7135,41 +7163,41 @@
       <c r="AV6" s="17"/>
     </row>
     <row r="7" spans="1:48" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="84" t="s">
+      <c r="B7" s="75" t="s">
         <v>284</v>
       </c>
-      <c r="C7" s="84"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="84"/>
-      <c r="H7" s="84"/>
-      <c r="I7" s="80" t="s">
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="75"/>
+      <c r="I7" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="J7" s="81"/>
-      <c r="K7" s="81"/>
-      <c r="L7" s="81"/>
-      <c r="M7" s="81"/>
-      <c r="N7" s="81"/>
-      <c r="O7" s="82"/>
-      <c r="P7" s="73" t="s">
+      <c r="J7" s="79"/>
+      <c r="K7" s="79"/>
+      <c r="L7" s="79"/>
+      <c r="M7" s="79"/>
+      <c r="N7" s="79"/>
+      <c r="O7" s="80"/>
+      <c r="P7" s="81" t="s">
         <v>285</v>
       </c>
-      <c r="Q7" s="74"/>
-      <c r="R7" s="74"/>
-      <c r="S7" s="74"/>
-      <c r="T7" s="75"/>
-      <c r="U7" s="83" t="s">
+      <c r="Q7" s="82"/>
+      <c r="R7" s="82"/>
+      <c r="S7" s="82"/>
+      <c r="T7" s="83"/>
+      <c r="U7" s="87" t="s">
         <v>287</v>
       </c>
-      <c r="V7" s="83"/>
-      <c r="W7" s="83"/>
-      <c r="X7" s="83"/>
+      <c r="V7" s="87"/>
+      <c r="W7" s="87"/>
+      <c r="X7" s="87"/>
       <c r="Y7" s="19"/>
     </row>
     <row r="8" spans="1:48" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="76" t="s">
+      <c r="A8" s="77" t="s">
         <v>288</v>
       </c>
       <c r="B8" s="16">
@@ -7315,7 +7343,7 @@
       </c>
     </row>
     <row r="9" spans="1:48" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="76"/>
+      <c r="A9" s="77"/>
       <c r="B9" s="17" t="s">
         <v>32</v>
       </c>
@@ -7409,41 +7437,41 @@
       <c r="AV9" s="17"/>
     </row>
     <row r="10" spans="1:48" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="84" t="s">
+      <c r="B10" s="75" t="s">
         <v>284</v>
       </c>
-      <c r="C10" s="84"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="84"/>
-      <c r="F10" s="84"/>
-      <c r="G10" s="84"/>
-      <c r="H10" s="84"/>
-      <c r="I10" s="80" t="s">
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="75"/>
+      <c r="I10" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="J10" s="81"/>
-      <c r="K10" s="81"/>
-      <c r="L10" s="81"/>
-      <c r="M10" s="81"/>
-      <c r="N10" s="81"/>
-      <c r="O10" s="82"/>
-      <c r="P10" s="73" t="s">
+      <c r="J10" s="79"/>
+      <c r="K10" s="79"/>
+      <c r="L10" s="79"/>
+      <c r="M10" s="79"/>
+      <c r="N10" s="79"/>
+      <c r="O10" s="80"/>
+      <c r="P10" s="81" t="s">
         <v>285</v>
       </c>
-      <c r="Q10" s="74"/>
-      <c r="R10" s="74"/>
-      <c r="S10" s="74"/>
-      <c r="T10" s="75"/>
-      <c r="U10" s="83" t="s">
+      <c r="Q10" s="82"/>
+      <c r="R10" s="82"/>
+      <c r="S10" s="82"/>
+      <c r="T10" s="83"/>
+      <c r="U10" s="87" t="s">
         <v>287</v>
       </c>
-      <c r="V10" s="83"/>
-      <c r="W10" s="83"/>
-      <c r="X10" s="83"/>
+      <c r="V10" s="87"/>
+      <c r="W10" s="87"/>
+      <c r="X10" s="87"/>
       <c r="Y10" s="19"/>
     </row>
     <row r="11" spans="1:48" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="76" t="s">
+      <c r="A11" s="77" t="s">
         <v>289</v>
       </c>
       <c r="B11" s="16">
@@ -7589,7 +7617,7 @@
       </c>
     </row>
     <row r="12" spans="1:48" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="76"/>
+      <c r="A12" s="77"/>
       <c r="B12" s="17" t="s">
         <v>32</v>
       </c>
@@ -7684,40 +7712,40 @@
     </row>
     <row r="14" spans="1:48" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="31"/>
-      <c r="C14" s="77" t="s">
+      <c r="C14" s="84" t="s">
         <v>284</v>
       </c>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="78"/>
-      <c r="H14" s="78"/>
-      <c r="I14" s="79"/>
-      <c r="J14" s="80" t="s">
+      <c r="D14" s="85"/>
+      <c r="E14" s="85"/>
+      <c r="F14" s="85"/>
+      <c r="G14" s="85"/>
+      <c r="H14" s="85"/>
+      <c r="I14" s="86"/>
+      <c r="J14" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="K14" s="81"/>
-      <c r="L14" s="81"/>
-      <c r="M14" s="81"/>
-      <c r="N14" s="81"/>
-      <c r="O14" s="81"/>
-      <c r="P14" s="81"/>
-      <c r="Q14" s="81"/>
-      <c r="R14" s="81"/>
-      <c r="S14" s="81"/>
-      <c r="T14" s="82"/>
-      <c r="U14" s="73" t="s">
+      <c r="K14" s="79"/>
+      <c r="L14" s="79"/>
+      <c r="M14" s="79"/>
+      <c r="N14" s="79"/>
+      <c r="O14" s="79"/>
+      <c r="P14" s="79"/>
+      <c r="Q14" s="79"/>
+      <c r="R14" s="79"/>
+      <c r="S14" s="79"/>
+      <c r="T14" s="80"/>
+      <c r="U14" s="81" t="s">
         <v>285</v>
       </c>
-      <c r="V14" s="74"/>
-      <c r="W14" s="75"/>
+      <c r="V14" s="82"/>
+      <c r="W14" s="83"/>
       <c r="X14" s="30" t="s">
         <v>287</v>
       </c>
       <c r="Y14" s="32"/>
     </row>
     <row r="15" spans="1:48" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="76" t="s">
+      <c r="A15" s="77" t="s">
         <v>309</v>
       </c>
       <c r="B15" s="16">
@@ -7794,7 +7822,7 @@
       </c>
     </row>
     <row r="16" spans="1:48" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="76"/>
+      <c r="A16" s="77"/>
       <c r="B16" s="17" t="s">
         <v>32</v>
       </c>
@@ -7875,6 +7903,16 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="U14:W14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="C14:I14"/>
+    <mergeCell ref="J14:T14"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="P7:T7"/>
+    <mergeCell ref="U7:X7"/>
+    <mergeCell ref="P10:T10"/>
+    <mergeCell ref="U10:X10"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="I1:M1"/>
     <mergeCell ref="B4:H4"/>
@@ -7886,16 +7924,6 @@
     <mergeCell ref="I7:O7"/>
     <mergeCell ref="I10:O10"/>
     <mergeCell ref="B10:H10"/>
-    <mergeCell ref="U14:W14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="C14:I14"/>
-    <mergeCell ref="J14:T14"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="N4:Q4"/>
-    <mergeCell ref="P7:T7"/>
-    <mergeCell ref="U7:X7"/>
-    <mergeCell ref="P10:T10"/>
-    <mergeCell ref="U10:X10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -7931,27 +7959,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="84" t="s">
+      <c r="B1" s="75" t="s">
         <v>284</v>
       </c>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="85" t="s">
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="76" t="s">
         <v>285</v>
       </c>
-      <c r="J1" s="85"/>
-      <c r="K1" s="85"/>
-      <c r="L1" s="85"/>
-      <c r="M1" s="85"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
       <c r="N1" s="25"/>
       <c r="O1" s="25"/>
     </row>
     <row r="2" spans="1:22" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="77" t="s">
         <v>292</v>
       </c>
       <c r="B2" s="16">
@@ -8003,7 +8031,7 @@
       <c r="T2" s="16"/>
     </row>
     <row r="3" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="76"/>
+      <c r="A3" s="77"/>
       <c r="B3" s="21" t="s">
         <v>28</v>
       </c>
@@ -8053,34 +8081,34 @@
       <c r="T3" s="17"/>
     </row>
     <row r="4" spans="1:22" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="75" t="s">
         <v>284</v>
       </c>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="80" t="s">
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="J4" s="81"/>
-      <c r="K4" s="81"/>
-      <c r="L4" s="81"/>
-      <c r="M4" s="81"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="79"/>
+      <c r="L4" s="79"/>
+      <c r="M4" s="79"/>
       <c r="N4" s="20"/>
       <c r="O4" s="20"/>
-      <c r="P4" s="73" t="s">
+      <c r="P4" s="81" t="s">
         <v>285</v>
       </c>
-      <c r="Q4" s="74"/>
-      <c r="R4" s="74"/>
-      <c r="S4" s="74"/>
-      <c r="T4" s="75"/>
+      <c r="Q4" s="82"/>
+      <c r="R4" s="82"/>
+      <c r="S4" s="82"/>
+      <c r="T4" s="83"/>
     </row>
     <row r="5" spans="1:22" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="76" t="s">
+      <c r="A5" s="77" t="s">
         <v>293</v>
       </c>
       <c r="B5" s="16">
@@ -8148,7 +8176,7 @@
       </c>
     </row>
     <row r="6" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="76"/>
+      <c r="A6" s="77"/>
       <c r="B6" s="21" t="s">
         <v>28</v>
       </c>
@@ -8214,34 +8242,34 @@
       </c>
     </row>
     <row r="7" spans="1:22" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="84" t="s">
+      <c r="B7" s="75" t="s">
         <v>284</v>
       </c>
-      <c r="C7" s="84"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="84"/>
-      <c r="H7" s="84"/>
-      <c r="I7" s="80" t="s">
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="75"/>
+      <c r="I7" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="J7" s="81"/>
-      <c r="K7" s="81"/>
-      <c r="L7" s="81"/>
-      <c r="M7" s="81"/>
+      <c r="J7" s="79"/>
+      <c r="K7" s="79"/>
+      <c r="L7" s="79"/>
+      <c r="M7" s="79"/>
       <c r="N7" s="20"/>
       <c r="O7" s="20"/>
-      <c r="P7" s="73" t="s">
+      <c r="P7" s="81" t="s">
         <v>285</v>
       </c>
-      <c r="Q7" s="74"/>
-      <c r="R7" s="74"/>
-      <c r="S7" s="74"/>
-      <c r="T7" s="75"/>
+      <c r="Q7" s="82"/>
+      <c r="R7" s="82"/>
+      <c r="S7" s="82"/>
+      <c r="T7" s="83"/>
     </row>
     <row r="8" spans="1:22" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="76" t="s">
+      <c r="A8" s="77" t="s">
         <v>294</v>
       </c>
       <c r="B8" s="16">
@@ -8309,7 +8337,7 @@
       </c>
     </row>
     <row r="9" spans="1:22" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="76"/>
+      <c r="A9" s="77"/>
       <c r="B9" s="39" t="s">
         <v>28</v>
       </c>
@@ -8386,17 +8414,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="P4:T4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="I7:M7"/>
+    <mergeCell ref="P7:T7"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="I1:M1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="I4:M4"/>
-    <mergeCell ref="P4:T4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="I7:M7"/>
-    <mergeCell ref="P7:T7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -8405,10 +8433,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="F16:G17"/>
+      <selection activeCell="B17" sqref="B17:M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8417,15 +8445,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="14" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:12" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="77" t="s">
         <v>299</v>
       </c>
       <c r="B2" s="16">
@@ -8455,7 +8483,7 @@
       <c r="L2" s="16"/>
     </row>
     <row r="3" spans="1:12" s="14" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="76"/>
+      <c r="A3" s="77"/>
       <c r="B3" s="21" t="s">
         <v>32</v>
       </c>
@@ -8502,7 +8530,7 @@
       <c r="L5" s="29"/>
     </row>
     <row r="6" spans="1:12" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="76" t="s">
+      <c r="A6" s="77" t="s">
         <v>301</v>
       </c>
       <c r="B6" s="16">
@@ -8540,7 +8568,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" s="14" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="76"/>
+      <c r="A7" s="77"/>
       <c r="B7" s="21" t="s">
         <v>28</v>
       </c>
@@ -8591,7 +8619,7 @@
       <c r="L11" s="29"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="76" t="s">
+      <c r="A12" s="77" t="s">
         <v>303</v>
       </c>
       <c r="B12" s="16">
@@ -8629,7 +8657,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="76"/>
+      <c r="A13" s="77"/>
       <c r="B13" s="21" t="s">
         <v>28</v>
       </c>
@@ -8650,12 +8678,107 @@
       <c r="K13" s="21"/>
       <c r="L13" s="21"/>
     </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="29"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="77" t="s">
+        <v>333</v>
+      </c>
+      <c r="B17" s="16">
+        <v>234</v>
+      </c>
+      <c r="C17" s="16">
+        <v>235</v>
+      </c>
+      <c r="D17" s="16">
+        <v>236</v>
+      </c>
+      <c r="E17" s="16">
+        <v>237</v>
+      </c>
+      <c r="F17" s="16">
+        <v>238</v>
+      </c>
+      <c r="G17" s="16">
+        <v>239</v>
+      </c>
+      <c r="H17" s="16">
+        <v>240</v>
+      </c>
+      <c r="I17" s="16">
+        <v>241</v>
+      </c>
+      <c r="J17" s="16">
+        <v>242</v>
+      </c>
+      <c r="K17" s="16">
+        <v>243</v>
+      </c>
+      <c r="L17" s="16">
+        <v>244</v>
+      </c>
+      <c r="M17" s="16">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="77"/>
+      <c r="B18" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="21">
+        <v>8</v>
+      </c>
+      <c r="D18" s="21">
+        <v>5</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="21">
+        <v>8</v>
+      </c>
+      <c r="H18" s="21">
+        <v>5</v>
+      </c>
+      <c r="I18" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="J18" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="K18" s="21">
+        <v>8</v>
+      </c>
+      <c r="L18" s="21">
+        <v>5</v>
+      </c>
+      <c r="M18" s="23" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A17:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8719,7 +8842,7 @@
       <c r="C2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="56" t="s">
+      <c r="D2" s="59" t="s">
         <v>54</v>
       </c>
       <c r="E2" s="6" t="str">
@@ -8744,7 +8867,7 @@
       <c r="C3" s="7">
         <v>1</v>
       </c>
-      <c r="D3" s="56"/>
+      <c r="D3" s="59"/>
       <c r="E3" s="6" t="str">
         <f t="shared" ref="E3:E66" si="0">IF(AND(B3=C3,B3&lt;&gt;" "),"OK","ERROR")</f>
         <v>OK</v>
@@ -8760,7 +8883,7 @@
       <c r="C4" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="56"/>
+      <c r="D4" s="59"/>
       <c r="E4" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -8776,7 +8899,7 @@
       <c r="C5" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="56" t="s">
+      <c r="D5" s="59" t="s">
         <v>54</v>
       </c>
       <c r="E5" s="6" t="str">
@@ -8794,7 +8917,7 @@
       <c r="C6" s="7">
         <v>10</v>
       </c>
-      <c r="D6" s="56"/>
+      <c r="D6" s="59"/>
       <c r="E6" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -8810,7 +8933,7 @@
       <c r="C7" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="56"/>
+      <c r="D7" s="59"/>
       <c r="E7" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -8826,7 +8949,7 @@
       <c r="C8" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="63" t="s">
+      <c r="D8" s="60" t="s">
         <v>280</v>
       </c>
       <c r="E8" s="6" t="str">
@@ -8844,7 +8967,7 @@
       <c r="C9" s="7">
         <v>15</v>
       </c>
-      <c r="D9" s="63"/>
+      <c r="D9" s="60"/>
       <c r="E9" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -8860,7 +8983,7 @@
       <c r="C10" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="63"/>
+      <c r="D10" s="60"/>
       <c r="E10" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -8876,7 +8999,7 @@
       <c r="C11" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="63"/>
+      <c r="D11" s="60"/>
       <c r="E11" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -8892,7 +9015,7 @@
       <c r="C12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="63"/>
+      <c r="D12" s="60"/>
       <c r="E12" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -8908,7 +9031,7 @@
       <c r="C13" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="63"/>
+      <c r="D13" s="60"/>
       <c r="E13" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -8924,7 +9047,7 @@
       <c r="C14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="63"/>
+      <c r="D14" s="60"/>
       <c r="E14" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -8940,7 +9063,7 @@
       <c r="C15" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="63"/>
+      <c r="D15" s="60"/>
       <c r="E15" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -8956,7 +9079,7 @@
       <c r="C16" s="7">
         <v>16</v>
       </c>
-      <c r="D16" s="63"/>
+      <c r="D16" s="60"/>
       <c r="E16" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -8972,7 +9095,7 @@
       <c r="C17" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="63"/>
+      <c r="D17" s="60"/>
       <c r="E17" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -8988,7 +9111,7 @@
       <c r="C18" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="63"/>
+      <c r="D18" s="60"/>
       <c r="E18" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9004,7 +9127,7 @@
       <c r="C19" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="63"/>
+      <c r="D19" s="60"/>
       <c r="E19" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9020,7 +9143,7 @@
       <c r="C20" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="58" t="s">
+      <c r="D20" s="61" t="s">
         <v>281</v>
       </c>
       <c r="E20" s="6" t="str">
@@ -9038,7 +9161,7 @@
       <c r="C21" s="7">
         <v>15</v>
       </c>
-      <c r="D21" s="59"/>
+      <c r="D21" s="62"/>
       <c r="E21" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9054,7 +9177,7 @@
       <c r="C22" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="59"/>
+      <c r="D22" s="62"/>
       <c r="E22" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9070,7 +9193,7 @@
       <c r="C23" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="59"/>
+      <c r="D23" s="62"/>
       <c r="E23" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9086,7 +9209,7 @@
       <c r="C24" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="59"/>
+      <c r="D24" s="62"/>
       <c r="E24" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9102,7 +9225,7 @@
       <c r="C25" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="59"/>
+      <c r="D25" s="62"/>
       <c r="E25" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9118,7 +9241,7 @@
       <c r="C26" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="59"/>
+      <c r="D26" s="62"/>
       <c r="E26" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9134,7 +9257,7 @@
       <c r="C27" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="59"/>
+      <c r="D27" s="62"/>
       <c r="E27" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9150,7 +9273,7 @@
       <c r="C28" s="7">
         <v>16</v>
       </c>
-      <c r="D28" s="59"/>
+      <c r="D28" s="62"/>
       <c r="E28" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9166,7 +9289,7 @@
       <c r="C29" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="59"/>
+      <c r="D29" s="62"/>
       <c r="E29" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9182,7 +9305,7 @@
       <c r="C30" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="59"/>
+      <c r="D30" s="62"/>
       <c r="E30" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9198,7 +9321,7 @@
       <c r="C31" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D31" s="59"/>
+      <c r="D31" s="62"/>
       <c r="E31" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9214,7 +9337,7 @@
       <c r="C32" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="59"/>
+      <c r="D32" s="62"/>
       <c r="E32" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9230,7 +9353,7 @@
       <c r="C33" s="7">
         <v>17</v>
       </c>
-      <c r="D33" s="59"/>
+      <c r="D33" s="62"/>
       <c r="E33" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9246,7 +9369,7 @@
       <c r="C34" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="59"/>
+      <c r="D34" s="62"/>
       <c r="E34" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9262,7 +9385,7 @@
       <c r="C35" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D35" s="63" t="s">
+      <c r="D35" s="60" t="s">
         <v>290</v>
       </c>
       <c r="E35" s="6" t="str">
@@ -9280,7 +9403,7 @@
       <c r="C36" s="7">
         <v>15</v>
       </c>
-      <c r="D36" s="64"/>
+      <c r="D36" s="63"/>
       <c r="E36" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9296,7 +9419,7 @@
       <c r="C37" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D37" s="64"/>
+      <c r="D37" s="63"/>
       <c r="E37" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9312,7 +9435,7 @@
       <c r="C38" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D38" s="64"/>
+      <c r="D38" s="63"/>
       <c r="E38" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9328,7 +9451,7 @@
       <c r="C39" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D39" s="64"/>
+      <c r="D39" s="63"/>
       <c r="E39" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9344,7 +9467,7 @@
       <c r="C40" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D40" s="64"/>
+      <c r="D40" s="63"/>
       <c r="E40" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9360,7 +9483,7 @@
       <c r="C41" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D41" s="64"/>
+      <c r="D41" s="63"/>
       <c r="E41" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9376,7 +9499,7 @@
       <c r="C42" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D42" s="64"/>
+      <c r="D42" s="63"/>
       <c r="E42" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9392,7 +9515,7 @@
       <c r="C43" s="7">
         <v>4</v>
       </c>
-      <c r="D43" s="64"/>
+      <c r="D43" s="63"/>
       <c r="E43" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9408,7 +9531,7 @@
       <c r="C44" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D44" s="64"/>
+      <c r="D44" s="63"/>
       <c r="E44" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9424,7 +9547,7 @@
       <c r="C45" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D45" s="64"/>
+      <c r="D45" s="63"/>
       <c r="E45" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9440,7 +9563,7 @@
       <c r="C46" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D46" s="64"/>
+      <c r="D46" s="63"/>
       <c r="E46" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9456,7 +9579,7 @@
       <c r="C47" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D47" s="64"/>
+      <c r="D47" s="63"/>
       <c r="E47" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9473,7 +9596,7 @@
       <c r="C48" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D48" s="64"/>
+      <c r="D48" s="63"/>
       <c r="E48" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9490,7 +9613,7 @@
       <c r="C49" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D49" s="64"/>
+      <c r="D49" s="63"/>
       <c r="E49" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9507,7 +9630,7 @@
       <c r="C50" s="7">
         <v>16</v>
       </c>
-      <c r="D50" s="64"/>
+      <c r="D50" s="63"/>
       <c r="E50" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9524,7 +9647,7 @@
       <c r="C51" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D51" s="64"/>
+      <c r="D51" s="63"/>
       <c r="E51" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9540,7 +9663,7 @@
       <c r="C52" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D52" s="64"/>
+      <c r="D52" s="63"/>
       <c r="E52" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9556,7 +9679,7 @@
       <c r="C53" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D53" s="64"/>
+      <c r="D53" s="63"/>
       <c r="E53" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9572,7 +9695,7 @@
       <c r="C54" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="D54" s="64"/>
+      <c r="D54" s="63"/>
       <c r="E54" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9588,7 +9711,7 @@
       <c r="C55" s="7">
         <v>17</v>
       </c>
-      <c r="D55" s="64"/>
+      <c r="D55" s="63"/>
       <c r="E55" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9604,7 +9727,7 @@
       <c r="C56" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D56" s="64"/>
+      <c r="D56" s="63"/>
       <c r="E56" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9620,7 +9743,7 @@
       <c r="C57" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D57" s="65" t="s">
+      <c r="D57" s="64" t="s">
         <v>291</v>
       </c>
       <c r="E57" s="6" t="str">
@@ -9638,7 +9761,7 @@
       <c r="C58" s="7">
         <v>15</v>
       </c>
-      <c r="D58" s="66"/>
+      <c r="D58" s="65"/>
       <c r="E58" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9654,7 +9777,7 @@
       <c r="C59" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D59" s="66"/>
+      <c r="D59" s="65"/>
       <c r="E59" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9670,7 +9793,7 @@
       <c r="C60" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D60" s="66"/>
+      <c r="D60" s="65"/>
       <c r="E60" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9686,7 +9809,7 @@
       <c r="C61" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D61" s="66"/>
+      <c r="D61" s="65"/>
       <c r="E61" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9702,7 +9825,7 @@
       <c r="C62" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D62" s="66"/>
+      <c r="D62" s="65"/>
       <c r="E62" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9718,7 +9841,7 @@
       <c r="C63" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D63" s="66"/>
+      <c r="D63" s="65"/>
       <c r="E63" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9734,7 +9857,7 @@
       <c r="C64" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D64" s="66"/>
+      <c r="D64" s="65"/>
       <c r="E64" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9750,7 +9873,7 @@
       <c r="C65" s="7">
         <v>4</v>
       </c>
-      <c r="D65" s="66"/>
+      <c r="D65" s="65"/>
       <c r="E65" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9766,7 +9889,7 @@
       <c r="C66" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D66" s="66"/>
+      <c r="D66" s="65"/>
       <c r="E66" s="6" t="str">
         <f t="shared" si="0"/>
         <v>OK</v>
@@ -9782,7 +9905,7 @@
       <c r="C67" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D67" s="66"/>
+      <c r="D67" s="65"/>
       <c r="E67" s="6" t="str">
         <f t="shared" ref="E67:E130" si="1">IF(AND(B67=C67,B67&lt;&gt;" "),"OK","ERROR")</f>
         <v>OK</v>
@@ -9798,7 +9921,7 @@
       <c r="C68" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D68" s="66"/>
+      <c r="D68" s="65"/>
       <c r="E68" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -9814,7 +9937,7 @@
       <c r="C69" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D69" s="66"/>
+      <c r="D69" s="65"/>
       <c r="E69" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -9830,7 +9953,7 @@
       <c r="C70" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D70" s="66"/>
+      <c r="D70" s="65"/>
       <c r="E70" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -9846,7 +9969,7 @@
       <c r="C71" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D71" s="66"/>
+      <c r="D71" s="65"/>
       <c r="E71" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -9862,7 +9985,7 @@
       <c r="C72" s="7">
         <v>16</v>
       </c>
-      <c r="D72" s="66"/>
+      <c r="D72" s="65"/>
       <c r="E72" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -9878,7 +10001,7 @@
       <c r="C73" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D73" s="66"/>
+      <c r="D73" s="65"/>
       <c r="E73" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -9894,7 +10017,7 @@
       <c r="C74" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D74" s="66"/>
+      <c r="D74" s="65"/>
       <c r="E74" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -9910,7 +10033,7 @@
       <c r="C75" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D75" s="66"/>
+      <c r="D75" s="65"/>
       <c r="E75" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -9926,7 +10049,7 @@
       <c r="C76" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D76" s="66"/>
+      <c r="D76" s="65"/>
       <c r="E76" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -9942,7 +10065,7 @@
       <c r="C77" s="7">
         <v>17</v>
       </c>
-      <c r="D77" s="66"/>
+      <c r="D77" s="65"/>
       <c r="E77" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -9958,7 +10081,7 @@
       <c r="C78" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D78" s="66"/>
+      <c r="D78" s="65"/>
       <c r="E78" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -9974,7 +10097,7 @@
       <c r="C79" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D79" s="57" t="s">
+      <c r="D79" s="89" t="s">
         <v>295</v>
       </c>
       <c r="E79" s="6" t="str">
@@ -9992,7 +10115,7 @@
       <c r="C80" s="7">
         <v>7</v>
       </c>
-      <c r="D80" s="57"/>
+      <c r="D80" s="89"/>
       <c r="E80" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10008,7 +10131,7 @@
       <c r="C81" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D81" s="57"/>
+      <c r="D81" s="89"/>
       <c r="E81" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10024,7 +10147,7 @@
       <c r="C82" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D82" s="57"/>
+      <c r="D82" s="89"/>
       <c r="E82" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10040,7 +10163,7 @@
       <c r="C83" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="D83" s="57"/>
+      <c r="D83" s="89"/>
       <c r="E83" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10056,7 +10179,7 @@
       <c r="C84" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D84" s="57"/>
+      <c r="D84" s="89"/>
       <c r="E84" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10072,7 +10195,7 @@
       <c r="C85" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="D85" s="57"/>
+      <c r="D85" s="89"/>
       <c r="E85" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10088,7 +10211,7 @@
       <c r="C86" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D86" s="57"/>
+      <c r="D86" s="89"/>
       <c r="E86" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10104,7 +10227,7 @@
       <c r="C87" s="7">
         <v>5</v>
       </c>
-      <c r="D87" s="57"/>
+      <c r="D87" s="89"/>
       <c r="E87" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10120,7 +10243,7 @@
       <c r="C88" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D88" s="57"/>
+      <c r="D88" s="89"/>
       <c r="E88" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10136,7 +10259,7 @@
       <c r="C89" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D89" s="57"/>
+      <c r="D89" s="89"/>
       <c r="E89" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10152,7 +10275,7 @@
       <c r="C90" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D90" s="57"/>
+      <c r="D90" s="89"/>
       <c r="E90" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10168,7 +10291,7 @@
       <c r="C91" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D91" s="58" t="s">
+      <c r="D91" s="61" t="s">
         <v>296</v>
       </c>
       <c r="E91" s="6" t="str">
@@ -10186,7 +10309,7 @@
       <c r="C92" s="7">
         <v>7</v>
       </c>
-      <c r="D92" s="59"/>
+      <c r="D92" s="62"/>
       <c r="E92" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10202,7 +10325,7 @@
       <c r="C93" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D93" s="59"/>
+      <c r="D93" s="62"/>
       <c r="E93" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10218,7 +10341,7 @@
       <c r="C94" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D94" s="59"/>
+      <c r="D94" s="62"/>
       <c r="E94" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10234,7 +10357,7 @@
       <c r="C95" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="D95" s="59"/>
+      <c r="D95" s="62"/>
       <c r="E95" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10250,7 +10373,7 @@
       <c r="C96" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D96" s="59"/>
+      <c r="D96" s="62"/>
       <c r="E96" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10266,7 +10389,7 @@
       <c r="C97" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="D97" s="59"/>
+      <c r="D97" s="62"/>
       <c r="E97" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10282,7 +10405,7 @@
       <c r="C98" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D98" s="59"/>
+      <c r="D98" s="62"/>
       <c r="E98" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10298,7 +10421,7 @@
       <c r="C99" s="7">
         <v>8</v>
       </c>
-      <c r="D99" s="59"/>
+      <c r="D99" s="62"/>
       <c r="E99" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10314,7 +10437,7 @@
       <c r="C100" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D100" s="59"/>
+      <c r="D100" s="62"/>
       <c r="E100" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10330,7 +10453,7 @@
       <c r="C101" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D101" s="59"/>
+      <c r="D101" s="62"/>
       <c r="E101" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10346,7 +10469,7 @@
       <c r="C102" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="D102" s="59"/>
+      <c r="D102" s="62"/>
       <c r="E102" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10362,7 +10485,7 @@
       <c r="C103" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D103" s="59"/>
+      <c r="D103" s="62"/>
       <c r="E103" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10378,7 +10501,7 @@
       <c r="C104" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="D104" s="59"/>
+      <c r="D104" s="62"/>
       <c r="E104" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10394,7 +10517,7 @@
       <c r="C105" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D105" s="59"/>
+      <c r="D105" s="62"/>
       <c r="E105" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10410,7 +10533,7 @@
       <c r="C106" s="7">
         <v>5</v>
       </c>
-      <c r="D106" s="59"/>
+      <c r="D106" s="62"/>
       <c r="E106" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10426,7 +10549,7 @@
       <c r="C107" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D107" s="59"/>
+      <c r="D107" s="62"/>
       <c r="E107" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10442,7 +10565,7 @@
       <c r="C108" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D108" s="59"/>
+      <c r="D108" s="62"/>
       <c r="E108" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10458,7 +10581,7 @@
       <c r="C109" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D109" s="60"/>
+      <c r="D109" s="90"/>
       <c r="E109" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10474,7 +10597,7 @@
       <c r="C110" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D110" s="61" t="s">
+      <c r="D110" s="72" t="s">
         <v>297</v>
       </c>
       <c r="E110" s="6" t="str">
@@ -10492,7 +10615,7 @@
       <c r="C111" s="7">
         <v>7</v>
       </c>
-      <c r="D111" s="61"/>
+      <c r="D111" s="72"/>
       <c r="E111" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10508,7 +10631,7 @@
       <c r="C112" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D112" s="61"/>
+      <c r="D112" s="72"/>
       <c r="E112" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10524,7 +10647,7 @@
       <c r="C113" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D113" s="61"/>
+      <c r="D113" s="72"/>
       <c r="E113" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10540,7 +10663,7 @@
       <c r="C114" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="D114" s="61"/>
+      <c r="D114" s="72"/>
       <c r="E114" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10556,7 +10679,7 @@
       <c r="C115" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D115" s="61"/>
+      <c r="D115" s="72"/>
       <c r="E115" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10572,7 +10695,7 @@
       <c r="C116" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D116" s="61"/>
+      <c r="D116" s="72"/>
       <c r="E116" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10588,7 +10711,7 @@
       <c r="C117" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D117" s="61"/>
+      <c r="D117" s="72"/>
       <c r="E117" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10604,7 +10727,7 @@
       <c r="C118" s="7">
         <v>8</v>
       </c>
-      <c r="D118" s="61"/>
+      <c r="D118" s="72"/>
       <c r="E118" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10620,7 +10743,7 @@
       <c r="C119" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D119" s="61"/>
+      <c r="D119" s="72"/>
       <c r="E119" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10636,7 +10759,7 @@
       <c r="C120" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D120" s="61"/>
+      <c r="D120" s="72"/>
       <c r="E120" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10652,7 +10775,7 @@
       <c r="C121" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D121" s="61"/>
+      <c r="D121" s="72"/>
       <c r="E121" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10668,7 +10791,7 @@
       <c r="C122" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D122" s="61"/>
+      <c r="D122" s="72"/>
       <c r="E122" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10684,7 +10807,7 @@
       <c r="C123" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D123" s="61"/>
+      <c r="D123" s="72"/>
       <c r="E123" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10700,7 +10823,7 @@
       <c r="C124" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D124" s="61"/>
+      <c r="D124" s="72"/>
       <c r="E124" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10716,7 +10839,7 @@
       <c r="C125" s="7">
         <v>5</v>
       </c>
-      <c r="D125" s="61"/>
+      <c r="D125" s="72"/>
       <c r="E125" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10732,7 +10855,7 @@
       <c r="C126" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D126" s="61"/>
+      <c r="D126" s="72"/>
       <c r="E126" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10748,7 +10871,7 @@
       <c r="C127" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D127" s="61"/>
+      <c r="D127" s="72"/>
       <c r="E127" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10764,7 +10887,7 @@
       <c r="C128" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D128" s="62"/>
+      <c r="D128" s="74"/>
       <c r="E128" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10780,7 +10903,7 @@
       <c r="C129" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D129" s="47" t="s">
+      <c r="D129" s="50" t="s">
         <v>302</v>
       </c>
       <c r="E129" s="6" t="str">
@@ -10798,7 +10921,7 @@
       <c r="C130" s="7">
         <v>8</v>
       </c>
-      <c r="D130" s="48"/>
+      <c r="D130" s="51"/>
       <c r="E130" s="6" t="str">
         <f t="shared" si="1"/>
         <v>OK</v>
@@ -10814,7 +10937,7 @@
       <c r="C131" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D131" s="48"/>
+      <c r="D131" s="51"/>
       <c r="E131" s="6" t="str">
         <f t="shared" ref="E131:E185" si="2">IF(AND(B131=C131,B131&lt;&gt;" "),"OK","ERROR")</f>
         <v>OK</v>
@@ -10830,7 +10953,7 @@
       <c r="C132" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D132" s="48"/>
+      <c r="D132" s="51"/>
       <c r="E132" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -10846,7 +10969,7 @@
       <c r="C133" s="7">
         <v>8</v>
       </c>
-      <c r="D133" s="48"/>
+      <c r="D133" s="51"/>
       <c r="E133" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -10862,7 +10985,7 @@
       <c r="C134" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D134" s="48"/>
+      <c r="D134" s="51"/>
       <c r="E134" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -10878,7 +11001,7 @@
       <c r="C135" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D135" s="48"/>
+      <c r="D135" s="51"/>
       <c r="E135" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -10894,7 +11017,7 @@
       <c r="C136" s="7">
         <v>8</v>
       </c>
-      <c r="D136" s="48"/>
+      <c r="D136" s="51"/>
       <c r="E136" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -10910,7 +11033,7 @@
       <c r="C137" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D137" s="49"/>
+      <c r="D137" s="52"/>
       <c r="E137" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -10926,7 +11049,7 @@
       <c r="C138" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D138" s="50" t="s">
+      <c r="D138" s="56" t="s">
         <v>307</v>
       </c>
       <c r="E138" s="6" t="str">
@@ -10944,7 +11067,7 @@
       <c r="C139" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D139" s="51"/>
+      <c r="D139" s="57"/>
       <c r="E139" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -10960,7 +11083,7 @@
       <c r="C140" s="7">
         <v>2</v>
       </c>
-      <c r="D140" s="51"/>
+      <c r="D140" s="57"/>
       <c r="E140" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -10976,7 +11099,7 @@
       <c r="C141" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D141" s="51"/>
+      <c r="D141" s="57"/>
       <c r="E141" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -10992,7 +11115,7 @@
       <c r="C142" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="D142" s="51"/>
+      <c r="D142" s="57"/>
       <c r="E142" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -11008,7 +11131,7 @@
       <c r="C143" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="D143" s="51"/>
+      <c r="D143" s="57"/>
       <c r="E143" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -11024,7 +11147,7 @@
       <c r="C144" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D144" s="51"/>
+      <c r="D144" s="57"/>
       <c r="E144" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -11040,7 +11163,7 @@
       <c r="C145" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="D145" s="51"/>
+      <c r="D145" s="57"/>
       <c r="E145" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -11056,7 +11179,7 @@
       <c r="C146" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D146" s="51"/>
+      <c r="D146" s="57"/>
       <c r="E146" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -11072,7 +11195,7 @@
       <c r="C147" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D147" s="51"/>
+      <c r="D147" s="57"/>
       <c r="E147" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -11088,7 +11211,7 @@
       <c r="C148" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D148" s="51"/>
+      <c r="D148" s="57"/>
       <c r="E148" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -11104,7 +11227,7 @@
       <c r="C149" s="7">
         <v>4</v>
       </c>
-      <c r="D149" s="51"/>
+      <c r="D149" s="57"/>
       <c r="E149" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -11120,7 +11243,7 @@
       <c r="C150" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D150" s="51"/>
+      <c r="D150" s="57"/>
       <c r="E150" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -11136,7 +11259,7 @@
       <c r="C151" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="D151" s="51"/>
+      <c r="D151" s="57"/>
       <c r="E151" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -11152,7 +11275,7 @@
       <c r="C152" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D152" s="51"/>
+      <c r="D152" s="57"/>
       <c r="E152" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -11168,7 +11291,7 @@
       <c r="C153" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="D153" s="51"/>
+      <c r="D153" s="57"/>
       <c r="E153" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -11184,7 +11307,7 @@
       <c r="C154" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="D154" s="51"/>
+      <c r="D154" s="57"/>
       <c r="E154" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -11200,7 +11323,7 @@
       <c r="C155" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D155" s="51"/>
+      <c r="D155" s="57"/>
       <c r="E155" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -11216,7 +11339,7 @@
       <c r="C156" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="D156" s="51"/>
+      <c r="D156" s="57"/>
       <c r="E156" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -11232,7 +11355,7 @@
       <c r="C157" s="7">
         <v>1</v>
       </c>
-      <c r="D157" s="51"/>
+      <c r="D157" s="57"/>
       <c r="E157" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -11248,7 +11371,7 @@
       <c r="C158" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D158" s="51"/>
+      <c r="D158" s="57"/>
       <c r="E158" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -11264,7 +11387,7 @@
       <c r="C159" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="D159" s="51"/>
+      <c r="D159" s="57"/>
       <c r="E159" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -11280,7 +11403,7 @@
       <c r="C160" s="35">
         <v>0</v>
       </c>
-      <c r="D160" s="52"/>
+      <c r="D160" s="58"/>
       <c r="E160" s="6" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -11296,7 +11419,7 @@
       <c r="C161" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D161" s="86" t="s">
+      <c r="D161" s="88" t="s">
         <v>310</v>
       </c>
       <c r="E161" s="6" t="str">
@@ -11314,7 +11437,7 @@
       <c r="C162" s="7">
         <v>2</v>
       </c>
-      <c r="D162" s="86"/>
+      <c r="D162" s="88"/>
       <c r="E162" s="6" t="str">
         <f t="shared" si="2"/>
         <v>ERROR</v>
@@ -11330,7 +11453,7 @@
       <c r="C163" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D163" s="86"/>
+      <c r="D163" s="88"/>
       <c r="E163" s="6" t="str">
         <f t="shared" si="2"/>
         <v>ERROR</v>
@@ -11346,7 +11469,7 @@
       <c r="C164" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D164" s="86"/>
+      <c r="D164" s="88"/>
       <c r="E164" s="6" t="str">
         <f t="shared" si="2"/>
         <v>ERROR</v>
@@ -11362,7 +11485,7 @@
       <c r="C165" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D165" s="86"/>
+      <c r="D165" s="88"/>
       <c r="E165" s="6" t="str">
         <f t="shared" si="2"/>
         <v>ERROR</v>
@@ -11378,7 +11501,7 @@
       <c r="C166" s="7">
         <v>2</v>
       </c>
-      <c r="D166" s="86"/>
+      <c r="D166" s="88"/>
       <c r="E166" s="6" t="str">
         <f t="shared" si="2"/>
         <v>ERROR</v>
@@ -11394,7 +11517,7 @@
       <c r="C167" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D167" s="86"/>
+      <c r="D167" s="88"/>
       <c r="E167" s="6" t="str">
         <f t="shared" si="2"/>
         <v>ERROR</v>
@@ -11410,7 +11533,7 @@
       <c r="C168" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D168" s="86"/>
+      <c r="D168" s="88"/>
       <c r="E168" s="6" t="str">
         <f t="shared" si="2"/>
         <v>ERROR</v>
@@ -11426,7 +11549,7 @@
       <c r="C169" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D169" s="86"/>
+      <c r="D169" s="88"/>
       <c r="E169" s="6" t="str">
         <f t="shared" si="2"/>
         <v>ERROR</v>
@@ -11442,7 +11565,7 @@
       <c r="C170" s="7">
         <v>10</v>
       </c>
-      <c r="D170" s="86"/>
+      <c r="D170" s="88"/>
       <c r="E170" s="6" t="str">
         <f t="shared" si="2"/>
         <v>ERROR</v>
@@ -11458,7 +11581,7 @@
       <c r="C171" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D171" s="86"/>
+      <c r="D171" s="88"/>
       <c r="E171" s="6" t="str">
         <f t="shared" si="2"/>
         <v>ERROR</v>
@@ -11474,7 +11597,7 @@
       <c r="C172" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="D172" s="86"/>
+      <c r="D172" s="88"/>
       <c r="E172" s="6" t="str">
         <f t="shared" si="2"/>
         <v>ERROR</v>
@@ -11490,7 +11613,7 @@
       <c r="C173" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="D173" s="86"/>
+      <c r="D173" s="88"/>
       <c r="E173" s="6" t="str">
         <f t="shared" si="2"/>
         <v>ERROR</v>
@@ -11506,7 +11629,7 @@
       <c r="C174" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D174" s="86"/>
+      <c r="D174" s="88"/>
       <c r="E174" s="6" t="str">
         <f t="shared" si="2"/>
         <v>ERROR</v>
@@ -11522,7 +11645,7 @@
       <c r="C175" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="D175" s="86"/>
+      <c r="D175" s="88"/>
       <c r="E175" s="6" t="str">
         <f t="shared" si="2"/>
         <v>ERROR</v>
@@ -11538,7 +11661,7 @@
       <c r="C176" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D176" s="86"/>
+      <c r="D176" s="88"/>
       <c r="E176" s="6" t="str">
         <f t="shared" si="2"/>
         <v>ERROR</v>
@@ -11554,7 +11677,7 @@
       <c r="C177" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D177" s="86"/>
+      <c r="D177" s="88"/>
       <c r="E177" s="6" t="str">
         <f t="shared" si="2"/>
         <v>ERROR</v>
@@ -11570,7 +11693,7 @@
       <c r="C178" s="7">
         <v>163</v>
       </c>
-      <c r="D178" s="86"/>
+      <c r="D178" s="88"/>
       <c r="E178" s="6" t="str">
         <f t="shared" si="2"/>
         <v>ERROR</v>
@@ -11583,7 +11706,7 @@
       <c r="B179" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D179" s="86"/>
+      <c r="D179" s="88"/>
       <c r="E179" s="6" t="str">
         <f t="shared" si="2"/>
         <v>ERROR</v>
@@ -11596,7 +11719,7 @@
       <c r="B180" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D180" s="86"/>
+      <c r="D180" s="88"/>
       <c r="E180" s="6" t="str">
         <f t="shared" si="2"/>
         <v>ERROR</v>
@@ -11609,7 +11732,7 @@
       <c r="B181" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="D181" s="86"/>
+      <c r="D181" s="88"/>
       <c r="E181" s="6" t="str">
         <f t="shared" si="2"/>
         <v>ERROR</v>
@@ -11622,7 +11745,7 @@
       <c r="B182" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D182" s="86"/>
+      <c r="D182" s="88"/>
       <c r="E182" s="6" t="str">
         <f t="shared" si="2"/>
         <v>ERROR</v>
@@ -11635,7 +11758,7 @@
       <c r="B183" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D183" s="86"/>
+      <c r="D183" s="88"/>
       <c r="E183" s="6" t="str">
         <f t="shared" si="2"/>
         <v>ERROR</v>
@@ -11648,7 +11771,7 @@
       <c r="B184" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="D184" s="86"/>
+      <c r="D184" s="88"/>
       <c r="E184" s="6" t="str">
         <f t="shared" si="2"/>
         <v>ERROR</v>
@@ -11661,7 +11784,7 @@
       <c r="B185" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D185" s="86"/>
+      <c r="D185" s="88"/>
       <c r="E185" s="6" t="str">
         <f t="shared" si="2"/>
         <v>ERROR</v>

</xml_diff>